<commit_message>
refine the test case constructor, use testCaseConfig object to replace a long list of test case related configuration
</commit_message>
<xml_diff>
--- a/config/Automation_Test_Suite.xlsx
+++ b/config/Automation_Test_Suite.xlsx
@@ -444,7 +444,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -484,7 +484,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>